<commit_message>
test: added more data in the excel fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/fixture-multi-sheet.xlsx
+++ b/tests/fixtures/fixture-multi-sheet.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -155,12 +155,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -191,20 +190,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3828125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="16.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="1" style="1" width="16.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -221,6 +219,22 @@
       </c>
       <c r="B2" s="3" t="n">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>